<commit_message>
Remain - Revise Flow
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/UI_REVISE_FEEDBACK_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/UI_REVISE_FEEDBACK_HISTORY_DATA.xlsx
@@ -367,7 +367,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -737,30 +737,296 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>2024-07-15</t>
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>45488.79296148397</v>
-      </c>
-      <c r="C14" t="inlineStr">
+        <v>45488.79296148148</v>
+      </c>
+      <c r="C14" s="6" t="inlineStr">
         <is>
           <t>193livessd</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="6" t="n">
         <v>45</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="6" t="n">
         <v>56</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14" s="6" t="n">
         <v>-11</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14" s="6" t="n">
         <v>5.79</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="n">
+        <v>45489.46580332176</v>
+      </c>
+      <c r="C15" s="6" t="inlineStr">
+        <is>
+          <t>193fghj</t>
+        </is>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B16" s="9" t="n">
+        <v>45489.46703162037</v>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>193dfghj</t>
+        </is>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B17" s="9" t="n">
+        <v>45489.47452182871</v>
+      </c>
+      <c r="C17" s="6" t="inlineStr">
+        <is>
+          <t>aas22</t>
+        </is>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="n">
+        <v>45489.47601700231</v>
+      </c>
+      <c r="C18" s="6" t="inlineStr">
+        <is>
+          <t>193jjer</t>
+        </is>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>83</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>-23</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B19" s="9" t="n">
+        <v>45489.54144825231</v>
+      </c>
+      <c r="C19" s="6" t="inlineStr">
+        <is>
+          <t>193vinodds</t>
+        </is>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>113</v>
+      </c>
+      <c r="F19" s="6" t="n">
+        <v>-53</v>
+      </c>
+      <c r="G19" s="6" t="n">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B20" s="9" t="n">
+        <v>45489.55096924768</v>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>193ert</t>
+        </is>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>116</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="F20" s="6" t="n">
+        <v>83</v>
+      </c>
+      <c r="G20" s="6" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B21" s="9" t="n">
+        <v>45489.5618215162</v>
+      </c>
+      <c r="C21" s="6" t="inlineStr">
+        <is>
+          <t>193sdsdd</t>
+        </is>
+      </c>
+      <c r="D21" s="6" t="n">
+        <v>116</v>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="F21" s="6" t="n">
+        <v>82</v>
+      </c>
+      <c r="G21" s="6" t="n">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B22" s="9" t="n">
+        <v>45489.57467228009</v>
+      </c>
+      <c r="C22" s="6" t="inlineStr"/>
+      <c r="D22" s="6" t="n">
+        <v>116</v>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="F22" s="6" t="n">
+        <v>82</v>
+      </c>
+      <c r="G22" s="6" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B23" s="9" t="n">
+        <v>45489.57619274306</v>
+      </c>
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>193lattest</t>
+        </is>
+      </c>
+      <c r="D23" s="6" t="n">
+        <v>116</v>
+      </c>
+      <c r="E23" s="6" t="n">
+        <v>114</v>
+      </c>
+      <c r="F23" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="6" t="n">
+        <v>4.46</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B24" s="9" t="n">
+        <v>45489.58621821759</v>
+      </c>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <t>193vinoddd</t>
+        </is>
+      </c>
+      <c r="D24" s="6" t="n">
+        <v>115</v>
+      </c>
+      <c r="E24" s="6" t="n">
+        <v>112</v>
+      </c>
+      <c r="F24" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G24" s="6" t="n">
+        <v>4.96</v>
       </c>
     </row>
   </sheetData>
@@ -1050,7 +1316,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1336,6 +1602,60 @@
       </c>
       <c r="G10" s="6" t="n">
         <v>0.23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B11" s="9" t="n">
+        <v>45489.59596949074</v>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>193livee</t>
+        </is>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>115</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>114</v>
+      </c>
+      <c r="F11" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="n">
+        <v>45489.60234038021</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>194ddsds</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>115</v>
+      </c>
+      <c r="E12" t="n">
+        <v>114</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>